<commit_message>
Update sensor alert pin
</commit_message>
<xml_diff>
--- a/constraints/physical_pinout.xlsx
+++ b/constraints/physical_pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TiferKing\Documents\GitHub\ypcb_00338_1p1_hack\constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE79ABB-2CB5-4BD2-92A2-389773FCE2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4355E9A3-587C-4F78-AB1B-0F3E619009A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="6135" windowWidth="14400" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="324">
   <si>
     <t>RESETN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1000,6 +1000,14 @@
   </si>
   <si>
     <t>R28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P25</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1059,68 +1067,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1399,7 +1346,7 @@
   <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3008,6 +2955,12 @@
       <c r="C59" t="s">
         <v>109</v>
       </c>
+      <c r="D59" t="s">
+        <v>322</v>
+      </c>
+      <c r="E59" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">

</xml_diff>